<commit_message>
el atrib para conocer el edo. de justificante es integer estado
</commit_message>
<xml_diff>
--- a/Datos/asistencia.xlsx
+++ b/Datos/asistencia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Documents\GitHub\iso\proyecto\Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D48A5A66-207B-4029-A167-C3DD0930D763}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F407F24D-FEFF-475A-A903-E726AADF2D39}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7245" xr2:uid="{AC6D7A93-2CAE-4333-9396-147BD4BDD461}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7245" xr2:uid="{AC6D7A93-2CAE-4333-9396-147BD4BDD461}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -478,8 +478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0B919CA-52AB-47D8-82EC-6082FA6CEB4A}">
   <dimension ref="A1:E903"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A887" workbookViewId="0">
-      <selection activeCell="B900" sqref="B900"/>
+    <sheetView tabSelected="1" topLeftCell="A886" workbookViewId="0">
+      <selection activeCell="B901" sqref="B901"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15785,11 +15785,17 @@
       </c>
     </row>
     <row r="901" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A901" s="2"/>
-      <c r="B901" s="3"/>
+      <c r="A901" s="2">
+        <v>900</v>
+      </c>
+      <c r="B901" s="3">
+        <v>43264</v>
+      </c>
       <c r="C901" s="5"/>
       <c r="D901" s="5"/>
-      <c r="E901" s="2"/>
+      <c r="E901" s="2">
+        <v>10</v>
+      </c>
     </row>
     <row r="902" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B902" s="3"/>

</xml_diff>

<commit_message>
cambio de formato en fechas
</commit_message>
<xml_diff>
--- a/Datos/asistencia.xlsx
+++ b/Datos/asistencia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Documents\GitHub\iso\proyecto\Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F407F24D-FEFF-475A-A903-E726AADF2D39}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{728B17E2-601C-4E01-B4BF-97351B8D9A0F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7245" xr2:uid="{AC6D7A93-2CAE-4333-9396-147BD4BDD461}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7245" xr2:uid="{AC6D7A93-2CAE-4333-9396-147BD4BDD461}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -478,7 +478,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0B919CA-52AB-47D8-82EC-6082FA6CEB4A}">
   <dimension ref="A1:E903"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A886" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A890" workbookViewId="0">
       <selection activeCell="B901" sqref="B901"/>
     </sheetView>
   </sheetViews>

</xml_diff>